<commit_message>
Fixing errors, tax type fix, with V.Á.
</commit_message>
<xml_diff>
--- a/CAFETERIA FEJLESZTÉS/WF_cafeteria.xlsx
+++ b/CAFETERIA FEJLESZTÉS/WF_cafeteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\szabopet\Desktop\CAFETERIA FEJLESZTÉS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Cafeteria_nyilatkoztatas\CAFETERIA FEJLESZTÉS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71374FC2-7338-4DBC-8A30-C5701196A47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815F9FDA-C4AF-4ED9-A223-331594A61B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="30" windowWidth="38640" windowHeight="15840" tabRatio="855" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WF steps" sheetId="79" r:id="rId1"/>
@@ -2599,8 +2599,8 @@
   <sheetPr codeName="Munka28"/>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2"/>
@@ -3184,9 +3184,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CCE615-4582-4153-BBF9-9DEE93983CDE}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="13.2"/>
@@ -3235,7 +3235,7 @@
       <c r="F2" s="55"/>
       <c r="G2" s="56"/>
     </row>
-    <row r="3" spans="1:7" ht="66">
+    <row r="3" spans="1:7" ht="79.2">
       <c r="A3" s="38" t="s">
         <v>112</v>
       </c>

</xml_diff>